<commit_message>
fix incorrect column db
</commit_message>
<xml_diff>
--- a/database/dbexcel.xlsx
+++ b/database/dbexcel.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ShopDoChoi\database\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Toystore\database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{BA099D43-A890-4DD1-99C2-2D53F1B710C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17DBFA89-B66B-47B7-86AB-05506D7B9336}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{A540A835-73B2-4D68-B4F1-6F85F72BCDF2}"/>
   </bookViews>
@@ -104,9 +104,6 @@
     <t>Note</t>
   </si>
   <si>
-    <t>Amout</t>
-  </si>
-  <si>
     <t>Username (Key)</t>
   </si>
   <si>
@@ -120,13 +117,16 @@
   </si>
   <si>
     <t>BillID (Key)</t>
+  </si>
+  <si>
+    <t>Amount</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -503,15 +503,15 @@
   <dimension ref="A1:K8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.09765625" customWidth="1"/>
+    <col min="1" max="1" width="19.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -531,27 +531,27 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:11">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C3" t="s">
         <v>23</v>
       </c>
-      <c r="C3" t="s">
+      <c r="E3" t="s">
         <v>24</v>
       </c>
-      <c r="E3" t="s">
+      <c r="G3" t="s">
         <v>25</v>
       </c>
-      <c r="G3" t="s">
+      <c r="I3" t="s">
         <v>26</v>
       </c>
-      <c r="I3" t="s">
-        <v>27</v>
-      </c>
       <c r="K3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
-    <row r="4" spans="1:11">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -565,13 +565,13 @@
         <v>6</v>
       </c>
       <c r="I4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="K4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:11">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>14</v>
       </c>
@@ -588,7 +588,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:11">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>19</v>
       </c>
@@ -605,7 +605,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:11">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>2</v>
       </c>
@@ -619,12 +619,12 @@
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:11">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="G8" t="s">
         <v>21</v>
       </c>
       <c r="I8" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>